<commit_message>
[fix]relase and validastion bugs
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientesv.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/expediente/InformeExpedientesv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5131EA4C-C960-42E4-AC5D-DAA5777AEF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2ED6D-6589-4237-A6D7-0B2304B6E283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15370" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>{{item.Compañia}}</t>
+  </si>
+  <si>
+    <t>{{item.Clave}}</t>
   </si>
   <si>
     <t>{{item.Entrega}}</t>
@@ -115,13 +118,7 @@
     </r>
   </si>
   <si>
-    <t>{{item.Area}}</t>
-  </si>
-  <si>
-    <t>{{item.Status}}</t>
-  </si>
-  <si>
-    <t>{{item.Study}}</t>
+    <t>{{item.NombreEstatus}}</t>
   </si>
 </sst>
 </file>
@@ -661,7 +658,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,7 +675,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -737,19 +734,19 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>